<commit_message>
tired of writing commit messages
</commit_message>
<xml_diff>
--- a/daveydark/src/buyers.xlsx
+++ b/daveydark/src/buyers.xlsx
@@ -1,31 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APEX -hackathon\.venv\APEX-Hackathon\daveydark\src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5F5942-02DF-4FB6-A859-B79AED76AD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9A432DC2-3924-495C-BD0C-BFB8C7B09848}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>email</t>
   </si>
@@ -39,6 +27,9 @@
     <t>latitude</t>
   </si>
   <si>
+    <t>longitude</t>
+  </si>
+  <si>
     <t>state</t>
   </si>
   <si>
@@ -48,69 +39,67 @@
     <t>phone</t>
   </si>
   <si>
+    <t>wishlist</t>
+  </si>
+  <si>
     <t>test_1@davey</t>
   </si>
   <si>
+    <t>davesh</t>
+  </si>
+  <si>
+    <t>qq</t>
+  </si>
+  <si>
+    <t>punjab</t>
+  </si>
+  <si>
+    <t>ferozpur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>test_2@cash</t>
   </si>
   <si>
+    <t>cashmerekey</t>
+  </si>
+  <si>
     <t>test_3@ekus</t>
   </si>
   <si>
+    <t>ekuspreet</t>
+  </si>
+  <si>
     <t>test_4@aachi</t>
   </si>
   <si>
+    <t xml:space="preserve">aachi </t>
+  </si>
+  <si>
     <t>test_5@jaggi</t>
   </si>
   <si>
-    <t>davesh</t>
-  </si>
-  <si>
-    <t>cashmerekey</t>
-  </si>
-  <si>
-    <t>ekuspreet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aachi </t>
-  </si>
-  <si>
     <t>juggi</t>
-  </si>
-  <si>
-    <t>qq</t>
-  </si>
-  <si>
-    <t>punjab</t>
-  </si>
-  <si>
-    <t>ferozpur</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>wishlist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -132,12 +121,12 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -149,15 +138,295 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -199,108 +468,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -308,7 +483,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -334,7 +509,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -386,16 +561,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -411,7 +598,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -442,32 +629,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C704F09-E389-401B-874B-6CF2FF66A7CA}">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="12.6328125"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" width="11.7265625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="9.26953125"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" width="10.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,30 +661,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>30.9142279</v>
@@ -513,24 +693,27 @@
         <v>74.653574500000005</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>1234567890</v>
       </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>30.9142279</v>
@@ -539,24 +722,27 @@
         <v>74.653574500000005</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>1234567890</v>
       </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>30.9142279</v>
@@ -565,24 +751,27 @@
         <v>74.653574500000005</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H4">
         <v>1234567890</v>
       </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>30.9142279</v>
@@ -591,24 +780,27 @@
         <v>74.653574500000005</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H5">
         <v>1234567890</v>
       </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
       <c r="D6">
         <v>30.9142279</v>
@@ -617,10 +809,10 @@
         <v>74.653574500000005</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H6">
         <v>1234567890</v>
@@ -628,12 +820,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{01B095E1-2E3D-453D-B108-BEA2DC3D9F46}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{A349188A-11BB-4E8B-AC9E-DA182441DF10}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{4A710607-50B0-4E9A-8D6C-CDE1396AE366}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{B70CEB06-A958-4D73-913D-9B2593AA5440}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{DD2A0F5F-79C9-4615-8776-87DDD99339B5}"/>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>